<commit_message>
Modificacion descripcion,puntos de extension, curso basico
</commit_message>
<xml_diff>
--- a/CU1.5 Ver Supervisor.xlsx
+++ b/CU1.5 Ver Supervisor.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Pos-condición</t>
   </si>
@@ -43,9 +43,6 @@
     <t>Estado</t>
   </si>
   <si>
-    <t>0001</t>
-  </si>
-  <si>
     <t>Versión</t>
   </si>
   <si>
@@ -67,9 +64,6 @@
     <t>CUD1.5</t>
   </si>
   <si>
-    <t>Se muestran en pantalla todos los datos del supervisor seleccionado.</t>
-  </si>
-  <si>
     <t>Coordinador</t>
   </si>
   <si>
@@ -82,7 +76,52 @@
     <t>Que el actor tenga los permisos necesarios para ver el registro.</t>
   </si>
   <si>
-    <t>El actor hace clic en el botón "Ver" en algún registro del listado de supervisores.</t>
+    <t>Se muestran en pantalla todos los datos del supervisor seleccionado incluyendo un botón "Volver"</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Condicion:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> El actor quiere ver el detalle de un supervisor. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Punto de extensión</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>: Paso 2.e del CU03 Administracion de Coordinadores: El actor hace clic en el botón "Ver" en algún registro del listado de Supervisores del formulario "Administración de Coordinadores".</t>
+    </r>
+  </si>
+  <si>
+    <t>El actor hace click en el botón "Volver"</t>
+  </si>
+  <si>
+    <t>El sistema cierra el formulario</t>
+  </si>
+  <si>
+    <t>0003</t>
   </si>
 </sst>
 </file>
@@ -181,7 +220,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -240,6 +279,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -549,10 +591,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:C2"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -565,7 +607,7 @@
     <row r="1" spans="1:5" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A1" s="20"/>
       <c r="B1" s="19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C1" s="18">
         <v>42897</v>
@@ -575,39 +617,39 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" s="22"/>
+        <v>12</v>
+      </c>
+      <c r="B2" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="23"/>
       <c r="D2" s="17"/>
       <c r="E2" s="17"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="22"/>
+        <v>11</v>
+      </c>
+      <c r="B3" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="23"/>
       <c r="D3" s="17"/>
       <c r="E3" s="17"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B4" s="11"/>
       <c r="C4" s="3"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="C5" s="9"/>
     </row>
@@ -625,7 +667,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C7" s="3"/>
     </row>
@@ -634,7 +676,7 @@
         <v>5</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C8" s="3"/>
     </row>
@@ -643,7 +685,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C9" s="3"/>
     </row>
@@ -654,59 +696,75 @@
       <c r="B10" s="11"/>
       <c r="C10" s="3"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
+    <row r="11" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A11" s="5"/>
+      <c r="B11" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="3"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B11" s="15"/>
-      <c r="C11" s="14"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="8">
-        <v>1</v>
-      </c>
-      <c r="B12" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="C12" s="12"/>
+      <c r="B12" s="15"/>
+      <c r="C12" s="14"/>
     </row>
     <row r="13" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A13" s="8">
+        <v>1</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="12"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="8">
         <v>2</v>
       </c>
-      <c r="B13" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="C13" s="12"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
+      <c r="B14" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="12"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="8">
+        <v>3</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" s="12"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B14" s="11"/>
-      <c r="C14" s="3"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="8"/>
-      <c r="B15" s="10"/>
-      <c r="C15" s="9"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="8"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="6"/>
+      <c r="B16" s="11"/>
+      <c r="C16" s="3"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="8"/>
+      <c r="B17" s="10"/>
+      <c r="C17" s="9"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="8"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="6"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B17" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C17" s="3"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B18" s="2"/>
+      <c r="B19" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" s="3"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B20" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>